<commit_message>
Added multiple choice (single and multi select), fixed excel generation
</commit_message>
<xml_diff>
--- a/API/pdf-manager/Student Form.xlsx
+++ b/API/pdf-manager/Student Form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Gender</t>
   </si>
   <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -46,19 +49,67 @@
     <t>Summer</t>
   </si>
   <si>
-    <t>radio.option 0</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Tired, Fever</t>
   </si>
   <si>
     <t>Joe</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Science</t>
   </si>
   <si>
     <t>Fall</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Headache, Itchy</t>
+  </si>
+  <si>
+    <t>Milo</t>
+  </si>
+  <si>
+    <t>Treats!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer
+</t>
+  </si>
+  <si>
+    <t>Itchy</t>
+  </si>
+  <si>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>Long walks</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Meghan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring
+</t>
+  </si>
+  <si>
+    <t>Tired</t>
   </si>
 </sst>
 </file>
@@ -390,21 +441,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,45 +475,120 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>